<commit_message>
Updated korkeakouluopinto excel sample file
</commit_message>
<xml_diff>
--- a/tarjonta-app-angular/app/resources/import/korkeakouluopinto.xlsx
+++ b/tarjonta-app-angular/app/resources/import/korkeakouluopinto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="8480" tabRatio="475"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27740" windowHeight="10840" tabRatio="475"/>
   </bookViews>
   <sheets>
     <sheet name="Koulutukset" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="126">
   <si>
     <t>Koulutuksen tunniste</t>
   </si>
@@ -174,9 +174,6 @@
     <t>VALMIS</t>
   </si>
   <si>
-    <t>oid1, oid2, oid3</t>
-  </si>
-  <si>
     <t>opintojakso a</t>
   </si>
   <si>
@@ -186,33 +183,12 @@
     <t>name in english</t>
   </si>
   <si>
-    <t>Aineopinnot</t>
-  </si>
-  <si>
     <t>120 op</t>
   </si>
   <si>
     <t>2015</t>
   </si>
   <si>
-    <t>fi, sv, en</t>
-  </si>
-  <si>
-    <t>Iltaopetus</t>
-  </si>
-  <si>
-    <t>Ohjattu opiskelu</t>
-  </si>
-  <si>
-    <t>Etäopetus</t>
-  </si>
-  <si>
-    <t>Antropologia</t>
-  </si>
-  <si>
-    <t>Avainsana 1, avainsana 2</t>
-  </si>
-  <si>
     <t>Matti Meikäläinen</t>
   </si>
   <si>
@@ -249,60 +225,33 @@
     <t>Lisätietoja...</t>
   </si>
   <si>
-    <t>oid4</t>
-  </si>
-  <si>
     <t>opintojakso b</t>
   </si>
   <si>
-    <t>Perusopinnot</t>
-  </si>
-  <si>
     <t>100 op</t>
   </si>
   <si>
-    <t>sv</t>
-  </si>
-  <si>
     <t>150 €</t>
   </si>
   <si>
-    <t>Päiväopetus</t>
-  </si>
-  <si>
     <t>PUUTTEELLINEN</t>
   </si>
   <si>
-    <t>oid5</t>
-  </si>
-  <si>
     <t>opintojakso c</t>
   </si>
   <si>
-    <t>Soveltavat opinnot</t>
-  </si>
-  <si>
     <t>60 op</t>
   </si>
   <si>
-    <t>oid6</t>
-  </si>
-  <si>
     <t>opintokokonaisuus abc</t>
   </si>
   <si>
     <t>300 op</t>
   </si>
   <si>
-    <t>fi</t>
-  </si>
-  <si>
     <t>opintojakso x</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
     <t>opintokokonaisuus xy</t>
   </si>
   <si>
@@ -363,9 +312,6 @@
     <t>Lisätietoja hakemisesta tai ilmoittautumisesta (en)</t>
   </si>
   <si>
-    <t>KORKEAKOULUOPINTO</t>
-  </si>
-  <si>
     <t>1.2.246.562.10.79875033395</t>
   </si>
   <si>
@@ -427,13 +373,43 @@
   </si>
   <si>
     <t>esim-haku-2</t>
+  </si>
+  <si>
+    <t>kieli_fi, kieli_sv, kieli_en</t>
+  </si>
+  <si>
+    <t>kieli_sv</t>
+  </si>
+  <si>
+    <t>opinnontyyppi_1</t>
+  </si>
+  <si>
+    <t>opetusmuoto_e</t>
+  </si>
+  <si>
+    <t>opetusaikakk_1</t>
+  </si>
+  <si>
+    <t>opetusaikakk_2</t>
+  </si>
+  <si>
+    <t>opetuspaikkakk_2</t>
+  </si>
+  <si>
+    <t>teemat_1</t>
+  </si>
+  <si>
+    <t>teemat_1, teemat_2</t>
+  </si>
+  <si>
+    <t>oppiaineetyleissivistava</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -459,6 +435,14 @@
       <color rgb="FF333333"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -477,8 +461,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -488,7 +475,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -767,7 +757,7 @@
   <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -923,326 +913,316 @@
     </row>
     <row r="2" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:48" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="H5"/>
-      <c r="J5" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="J5" s="5"/>
       <c r="K5" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="P5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="P6" s="1"/>
       <c r="R6" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>59</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="J7" s="4"/>
       <c r="L7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="J8" s="4"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1230,7 @@
     <hyperlink ref="Y2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1259,7 +1239,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1269,134 +1249,134 @@
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="K2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="L2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="N2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="O2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="P2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="Q2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="R2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="S2" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>